<commit_message>
Updated Lookup tables with symbol changes
</commit_message>
<xml_diff>
--- a/DAS5/lookup_tables/instrumentsLookup.xlsx
+++ b/DAS5/lookup_tables/instrumentsLookup.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rajesh\Documents\Personal\DAS\DAS5\lookup_tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99BA8EEB-ABFA-48BA-A011-09D85F434DE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CD4497F-2FEB-46BB-B49F-B9B5284A4318}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="198">
   <si>
     <t>Symbol</t>
   </si>
@@ -221,9 +221,6 @@
   </si>
   <si>
     <t>EQUITASBNK</t>
-  </si>
-  <si>
-    <t>EQUITAS</t>
   </si>
   <si>
     <t>ENGINERSIN</t>
@@ -979,10 +976,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B191"/>
+  <dimension ref="A1:B190"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A177" workbookViewId="0">
-      <selection activeCell="G188" sqref="G188"/>
+    <sheetView tabSelected="1" topLeftCell="A168" workbookViewId="0">
+      <selection activeCell="H182" sqref="H182"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1445,1073 +1442,1065 @@
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B58" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B59" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B60" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B61" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B62" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B63" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B64" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B65" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B66" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B67" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B68" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B69" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B70" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B71" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B72" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B73" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B74" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B75" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B76" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B77" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B78" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B79" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B80" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B81" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B82" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B83" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B84" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B85" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B86" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B87" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B88" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B89" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B90" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B91" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B92" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B93" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B94" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B95" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B96" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B97" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B98" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B99" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B100" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B101" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B102" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B103" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B104" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B105" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B106" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B107" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B108" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B109" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B110" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B111" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B112" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B113" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B114" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B115" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B116" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B117" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B118" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B119" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B120" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B121" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B122" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B123" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B124" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B125" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B126" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B127" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B128" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B129" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B130" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B131" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B132" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B133" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B134" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B135" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B136" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B137" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B138" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B139" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B140" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B141" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B142" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B143" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B144" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B145" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B146" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B147" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B148" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B149" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B150" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B151" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B152" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B153" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B154" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B155" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B156" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B157" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B158" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B159" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B160" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B161" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B162" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B163" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B164" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B165" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B166" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B167" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B168" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B169" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B170" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B171" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B172" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B173" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B174" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B175" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B176" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B177" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B178" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B179" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A180" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B180" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B181" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B182" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A183" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B183" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A184" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B184" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A185" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B185" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A186" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B186" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A187" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B187" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A188" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B188" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A189" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B189" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A190" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B190" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="191" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A191" t="s">
-        <v>63</v>
-      </c>
-      <c r="B191" t="s">
         <v>63</v>
       </c>
     </row>

</xml_diff>